<commit_message>
code: make it better (untested)🤝
</commit_message>
<xml_diff>
--- a/protocol_database/diet.xlsx
+++ b/protocol_database/diet.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,6 +543,110 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ragu</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.6830000000000001</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.6830000000000001</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>[{"name": "Diet Base", "total": {"protein": 0, "calories": 0, "cost": 0.0, "amount": 0.0, "name": []}}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ragu</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0.6830000000000001</v>
+      </c>
+      <c r="D6" t="n">
+        <v>6</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.6830000000000001</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>[{"name": "Diet Base", "total": {"protein": 0, "calories": 0, "cost": 0.0, "amount": 0.0, "name": []}}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ragu</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>3.08716</v>
+      </c>
+      <c r="D7" t="n">
+        <v>27.12</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3.08716</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>[{"name": "Diet Base", "total": {"protein": 0, "calories": 0, "cost": 0.0, "amount": 0.0, "name": []}}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ragu</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1.92606</v>
+      </c>
+      <c r="D8" t="n">
+        <v>16.92</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.92606</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>[{"name": "Diet Base", "total": {"protein": 0, "calories": 0, "cost": 0.0, "amount": 0.0, "name": []}}]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>